<commit_message>
Trying full analysis data gen
</commit_message>
<xml_diff>
--- a/doc/Analysis.xlsx
+++ b/doc/Analysis.xlsx
@@ -8,19 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/work/qsm/maptester/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF31042-7FED-FE44-8BF8-AF5A061B31D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25626CBC-3FBE-DA4D-B356-DEA1B9021CFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57060" yWindow="-26120" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{52417819-FD4D-004A-80FD-AEA45B2BEE11}"/>
+    <workbookView xWindow="32680" yWindow="-25740" windowWidth="32460" windowHeight="20320" activeTab="4" xr2:uid="{52417819-FD4D-004A-80FD-AEA45B2BEE11}"/>
   </bookViews>
   <sheets>
     <sheet name="InitSize 75%" sheetId="2" r:id="rId1"/>
     <sheet name="InitSize 10%" sheetId="4" r:id="rId2"/>
     <sheet name="InitSize 5% same read" sheetId="5" r:id="rId3"/>
+    <sheet name="where good" sheetId="6" r:id="rId4"/>
+    <sheet name="sync map best" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="map_03_03_2097152_2020_03_16_23_59_06" localSheetId="3">'where good'!$A$1:$O$26</definedName>
     <definedName name="map_03_03_4194304_2020_03_16_22_24_52" localSheetId="0">'InitSize 75%'!$A$1:$M$37</definedName>
     <definedName name="map_03_03_4194304_2020_03_16_22_53_43" localSheetId="1">'InitSize 10%'!$A$1:$M$37</definedName>
     <definedName name="map_03_03_4194304_2020_03_16_23_08_54" localSheetId="2">'InitSize 5% same read'!$A$1:$M$37</definedName>
+    <definedName name="map_03_04_2097152_2020_03_17_00_16_21" localSheetId="4">'sync map best'!$A$1:$O$34</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +45,28 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{21F95336-64B8-7548-B6E0-451EC5CA2946}" name="map-03-03-4194304-2020-03-16_22_24_52" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="1" xr16:uid="{3385CFAE-DF07-9B46-BF0C-EE0E310030E4}" name="map-03-03-2097152-2020-03-16_23_59_06" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/System/Volumes/Data/work/qsm/maptester/build/perf/map-03-03-2097152-2020-03-16_23_59_06.csv" semicolon="1">
+      <textFields count="15">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" xr16:uid="{21F95336-64B8-7548-B6E0-451EC5CA2946}" name="map-03-03-4194304-2020-03-16_22_24_52" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="10000" sourceFile="/System/Volumes/Data/work/qsm/maptester/build/perf/map-03-03-4194304-2020-03-16_22_24_52.csv" semicolon="1">
       <textFields count="13">
         <textField/>
@@ -60,7 +85,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" xr16:uid="{D47B5A4C-D0AE-2342-93F3-072E1CB38770}" name="map-03-03-4194304-2020-03-16_22_53_43" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="3" xr16:uid="{D47B5A4C-D0AE-2342-93F3-072E1CB38770}" name="map-03-03-4194304-2020-03-16_22_53_43" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="10000" sourceFile="/System/Volumes/Data/work/qsm/maptester/build/perf/map-03-03-4194304-2020-03-16_22_53_43.csv" semicolon="1">
       <textFields count="13">
         <textField/>
@@ -79,9 +104,30 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" xr16:uid="{F26D10ED-958C-3D43-9BBB-848C033EABC0}" name="map-03-03-4194304-2020-03-16_23_08_54" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="4" xr16:uid="{F26D10ED-958C-3D43-9BBB-848C033EABC0}" name="map-03-03-4194304-2020-03-16_23_08_54" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="10000" sourceFile="/System/Volumes/Data/work/qsm/maptester/build/perf/map-03-03-4194304-2020-03-16_23_08_54.csv" semicolon="1">
       <textFields count="13">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" xr16:uid="{EA86C7E5-9CAD-2648-8952-3D78B8A90D02}" name="map-03-04-2097152-2020-03-17_00_16_21" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/System/Volumes/Data/work/qsm/maptester/build/perf/map-03-04-2097152-2020-03-17_00_16_21.csv" semicolon="1">
+      <textFields count="15">
+        <textField/>
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
@@ -102,7 +148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="22">
   <si>
     <t>Idx</t>
   </si>
@@ -156,6 +202,18 @@
   </si>
   <si>
     <t>25conflicts3d</t>
+  </si>
+  <si>
+    <t>init ratio</t>
+  </si>
+  <si>
+    <t>percent miss</t>
+  </si>
+  <si>
+    <t>50conflicts3d</t>
+  </si>
+  <si>
+    <t>perf</t>
   </si>
 </sst>
 </file>
@@ -211,15 +269,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="map-03-03-4194304-2020-03-16_22_24_52" connectionId="1" xr16:uid="{80106519-774E-E94F-87EA-F32E956369DE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="map-03-03-4194304-2020-03-16_22_24_52" connectionId="2" xr16:uid="{80106519-774E-E94F-87EA-F32E956369DE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="map-03-03-4194304-2020-03-16_22_53_43" connectionId="2" xr16:uid="{730C5190-B0A2-9547-8350-0E9A8BE590BB}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="map-03-03-4194304-2020-03-16_22_53_43" connectionId="3" xr16:uid="{730C5190-B0A2-9547-8350-0E9A8BE590BB}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="map-03-03-4194304-2020-03-16_23_08_54" connectionId="3" xr16:uid="{BFDC0E71-9746-034E-9A71-8E1438B57300}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="map-03-03-4194304-2020-03-16_23_08_54" connectionId="4" xr16:uid="{BFDC0E71-9746-034E-9A71-8E1438B57300}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="map-03-03-2097152-2020-03-16_23_59_06" connectionId="1" xr16:uid="{CFA56ABE-AB93-A94B-811A-C6F28FBBE79D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="map-03-04-2097152-2020-03-17_00_16_21" connectionId="5" xr16:uid="{1FCDD593-AA4C-404D-87A0-097DE755B6F9}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3707,8 +3773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEF630E4-0C6B-7D47-81E7-15AB4D267AE6}">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5294,4 +5360,2950 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1FAC4B6-0A46-814B-86D1-771DD8E31094}">
+  <dimension ref="A1:O26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2">
+        <v>2097152</v>
+      </c>
+      <c r="E2">
+        <v>2097152</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+      <c r="G2">
+        <v>0.3</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>64</v>
+      </c>
+      <c r="J2">
+        <v>8388608</v>
+      </c>
+      <c r="K2">
+        <v>4211053</v>
+      </c>
+      <c r="L2">
+        <v>338453448</v>
+      </c>
+      <c r="M2">
+        <v>2</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f>K2/(J2+D2)</f>
+        <v>0.40159730911254882</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>2097152</v>
+      </c>
+      <c r="E3">
+        <v>1898088</v>
+      </c>
+      <c r="F3">
+        <v>0.1</v>
+      </c>
+      <c r="G3">
+        <v>0.3</v>
+      </c>
+      <c r="H3">
+        <v>8</v>
+      </c>
+      <c r="I3">
+        <v>64</v>
+      </c>
+      <c r="J3">
+        <v>8388608</v>
+      </c>
+      <c r="K3">
+        <v>4944883</v>
+      </c>
+      <c r="L3">
+        <v>602478432</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f>K3/(J3+D3)</f>
+        <v>0.47158079147338866</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>2097152</v>
+      </c>
+      <c r="E4">
+        <v>1898088</v>
+      </c>
+      <c r="F4">
+        <v>0.1</v>
+      </c>
+      <c r="G4">
+        <v>0.3</v>
+      </c>
+      <c r="H4">
+        <v>32</v>
+      </c>
+      <c r="I4">
+        <v>64</v>
+      </c>
+      <c r="J4">
+        <v>8388608</v>
+      </c>
+      <c r="K4">
+        <v>5052844</v>
+      </c>
+      <c r="L4">
+        <v>338311072</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <f>K4/(J4+D4)</f>
+        <v>0.48187675476074221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>2097152</v>
+      </c>
+      <c r="E5">
+        <v>1637958</v>
+      </c>
+      <c r="F5">
+        <v>0.1</v>
+      </c>
+      <c r="G5">
+        <v>0.3</v>
+      </c>
+      <c r="H5">
+        <v>16</v>
+      </c>
+      <c r="I5">
+        <v>64</v>
+      </c>
+      <c r="J5">
+        <v>8388608</v>
+      </c>
+      <c r="K5">
+        <v>5090711</v>
+      </c>
+      <c r="L5">
+        <v>442510336</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f>K5/(J5+D5)</f>
+        <v>0.48548803329467771</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>2097152</v>
+      </c>
+      <c r="E6">
+        <v>1898088</v>
+      </c>
+      <c r="F6">
+        <v>0.1</v>
+      </c>
+      <c r="G6">
+        <v>0.3</v>
+      </c>
+      <c r="H6">
+        <v>64</v>
+      </c>
+      <c r="I6">
+        <v>64</v>
+      </c>
+      <c r="J6">
+        <v>8388608</v>
+      </c>
+      <c r="K6">
+        <v>5103023</v>
+      </c>
+      <c r="L6">
+        <v>338242080</v>
+      </c>
+      <c r="M6">
+        <v>2</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f>K6/(J6+D6)</f>
+        <v>0.4866621971130371</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>2097152</v>
+      </c>
+      <c r="E7">
+        <v>2097152</v>
+      </c>
+      <c r="F7">
+        <v>0.1</v>
+      </c>
+      <c r="G7">
+        <v>0.3</v>
+      </c>
+      <c r="H7">
+        <v>64</v>
+      </c>
+      <c r="I7">
+        <v>64</v>
+      </c>
+      <c r="J7">
+        <v>8388608</v>
+      </c>
+      <c r="K7">
+        <v>5172353</v>
+      </c>
+      <c r="L7">
+        <v>398821040</v>
+      </c>
+      <c r="M7">
+        <v>2</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f>K7/(J7+D7)</f>
+        <v>0.49327402114868163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>2097152</v>
+      </c>
+      <c r="E8">
+        <v>2097152</v>
+      </c>
+      <c r="F8">
+        <v>0.1</v>
+      </c>
+      <c r="G8">
+        <v>0.3</v>
+      </c>
+      <c r="H8">
+        <v>8</v>
+      </c>
+      <c r="I8">
+        <v>64</v>
+      </c>
+      <c r="J8">
+        <v>8388608</v>
+      </c>
+      <c r="K8">
+        <v>5234253</v>
+      </c>
+      <c r="L8">
+        <v>612440112</v>
+      </c>
+      <c r="M8">
+        <v>2</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f>K8/(J8+D8)</f>
+        <v>0.49917726516723632</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>2097152</v>
+      </c>
+      <c r="E9">
+        <v>1637958</v>
+      </c>
+      <c r="F9">
+        <v>0.1</v>
+      </c>
+      <c r="G9">
+        <v>0.3</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9">
+        <v>64</v>
+      </c>
+      <c r="J9">
+        <v>8388608</v>
+      </c>
+      <c r="K9">
+        <v>5249603</v>
+      </c>
+      <c r="L9">
+        <v>491471216</v>
+      </c>
+      <c r="M9">
+        <v>2</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f>K9/(J9+D9)</f>
+        <v>0.50064115524291997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>2097152</v>
+      </c>
+      <c r="E10">
+        <v>1637958</v>
+      </c>
+      <c r="F10">
+        <v>0.1</v>
+      </c>
+      <c r="G10">
+        <v>0.3</v>
+      </c>
+      <c r="H10">
+        <v>64</v>
+      </c>
+      <c r="I10">
+        <v>64</v>
+      </c>
+      <c r="J10">
+        <v>8388608</v>
+      </c>
+      <c r="K10">
+        <v>5286209</v>
+      </c>
+      <c r="L10">
+        <v>184778432</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f>K10/(J10+D10)</f>
+        <v>0.50413217544555666</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11">
+        <v>2097152</v>
+      </c>
+      <c r="E11">
+        <v>1898088</v>
+      </c>
+      <c r="F11">
+        <v>0.1</v>
+      </c>
+      <c r="G11">
+        <v>0.3</v>
+      </c>
+      <c r="H11">
+        <v>16</v>
+      </c>
+      <c r="I11">
+        <v>64</v>
+      </c>
+      <c r="J11">
+        <v>8388608</v>
+      </c>
+      <c r="K11">
+        <v>5357702</v>
+      </c>
+      <c r="L11">
+        <v>338392960</v>
+      </c>
+      <c r="M11">
+        <v>2</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f>K11/(J11+D11)</f>
+        <v>0.5109502792358398</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <v>2097152</v>
+      </c>
+      <c r="E12">
+        <v>1637958</v>
+      </c>
+      <c r="F12">
+        <v>0.1</v>
+      </c>
+      <c r="G12">
+        <v>0.3</v>
+      </c>
+      <c r="H12">
+        <v>32</v>
+      </c>
+      <c r="I12">
+        <v>64</v>
+      </c>
+      <c r="J12">
+        <v>8388608</v>
+      </c>
+      <c r="K12">
+        <v>5371127</v>
+      </c>
+      <c r="L12">
+        <v>367588080</v>
+      </c>
+      <c r="M12">
+        <v>2</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f>K12/(J12+D12)</f>
+        <v>0.51223058700561519</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13">
+        <v>2097152</v>
+      </c>
+      <c r="E13">
+        <v>2097152</v>
+      </c>
+      <c r="F13">
+        <v>0.1</v>
+      </c>
+      <c r="G13">
+        <v>0.3</v>
+      </c>
+      <c r="H13">
+        <v>8</v>
+      </c>
+      <c r="I13">
+        <v>64</v>
+      </c>
+      <c r="J13">
+        <v>8388608</v>
+      </c>
+      <c r="K13">
+        <v>5411763</v>
+      </c>
+      <c r="L13">
+        <v>338577232</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f>K13/(J13+D13)</f>
+        <v>0.51610593795776372</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14">
+        <v>2097152</v>
+      </c>
+      <c r="E14">
+        <v>2097152</v>
+      </c>
+      <c r="F14">
+        <v>0.1</v>
+      </c>
+      <c r="G14">
+        <v>0.3</v>
+      </c>
+      <c r="H14">
+        <v>32</v>
+      </c>
+      <c r="I14">
+        <v>64</v>
+      </c>
+      <c r="J14">
+        <v>8388608</v>
+      </c>
+      <c r="K14">
+        <v>5420608</v>
+      </c>
+      <c r="L14">
+        <v>338342944</v>
+      </c>
+      <c r="M14">
+        <v>2</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f>K14/(J14+D14)</f>
+        <v>0.51694946289062504</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15">
+        <v>2097152</v>
+      </c>
+      <c r="E15">
+        <v>1898088</v>
+      </c>
+      <c r="F15">
+        <v>0.1</v>
+      </c>
+      <c r="G15">
+        <v>0.3</v>
+      </c>
+      <c r="H15">
+        <v>8</v>
+      </c>
+      <c r="I15">
+        <v>64</v>
+      </c>
+      <c r="J15">
+        <v>8388608</v>
+      </c>
+      <c r="K15">
+        <v>5424187</v>
+      </c>
+      <c r="L15">
+        <v>338420320</v>
+      </c>
+      <c r="M15">
+        <v>2</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f>K15/(J15+D15)</f>
+        <v>0.51729078292846675</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>2097152</v>
+      </c>
+      <c r="E16">
+        <v>1637958</v>
+      </c>
+      <c r="F16">
+        <v>0.1</v>
+      </c>
+      <c r="G16">
+        <v>0.3</v>
+      </c>
+      <c r="H16">
+        <v>32</v>
+      </c>
+      <c r="I16">
+        <v>64</v>
+      </c>
+      <c r="J16">
+        <v>8388608</v>
+      </c>
+      <c r="K16">
+        <v>5424731</v>
+      </c>
+      <c r="L16">
+        <v>184743104</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f>K16/(J16+D16)</f>
+        <v>0.51734266281127927</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17">
+        <v>2097152</v>
+      </c>
+      <c r="E17">
+        <v>2097152</v>
+      </c>
+      <c r="F17">
+        <v>0.1</v>
+      </c>
+      <c r="G17">
+        <v>0.3</v>
+      </c>
+      <c r="H17">
+        <v>16</v>
+      </c>
+      <c r="I17">
+        <v>64</v>
+      </c>
+      <c r="J17">
+        <v>8388608</v>
+      </c>
+      <c r="K17">
+        <v>5425310</v>
+      </c>
+      <c r="L17">
+        <v>338416352</v>
+      </c>
+      <c r="M17">
+        <v>2</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f>K17/(J17+D17)</f>
+        <v>0.51739788055419922</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18">
+        <v>2097152</v>
+      </c>
+      <c r="E18">
+        <v>1898088</v>
+      </c>
+      <c r="F18">
+        <v>0.1</v>
+      </c>
+      <c r="G18">
+        <v>0.3</v>
+      </c>
+      <c r="H18">
+        <v>64</v>
+      </c>
+      <c r="I18">
+        <v>64</v>
+      </c>
+      <c r="J18">
+        <v>8388608</v>
+      </c>
+      <c r="K18">
+        <v>5426832</v>
+      </c>
+      <c r="L18">
+        <v>393982720</v>
+      </c>
+      <c r="M18">
+        <v>2</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <f>K18/(J18+D18)</f>
+        <v>0.51754302978515621</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19">
+        <v>2097152</v>
+      </c>
+      <c r="E19">
+        <v>1637958</v>
+      </c>
+      <c r="F19">
+        <v>0.1</v>
+      </c>
+      <c r="G19">
+        <v>0.3</v>
+      </c>
+      <c r="H19">
+        <v>8</v>
+      </c>
+      <c r="I19">
+        <v>64</v>
+      </c>
+      <c r="J19">
+        <v>8388608</v>
+      </c>
+      <c r="K19">
+        <v>5427117</v>
+      </c>
+      <c r="L19">
+        <v>184682048</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <f>K19/(J19+D19)</f>
+        <v>0.51757020950317378</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20">
+        <v>2097152</v>
+      </c>
+      <c r="E20">
+        <v>1898088</v>
+      </c>
+      <c r="F20">
+        <v>0.1</v>
+      </c>
+      <c r="G20">
+        <v>0.3</v>
+      </c>
+      <c r="H20">
+        <v>16</v>
+      </c>
+      <c r="I20">
+        <v>64</v>
+      </c>
+      <c r="J20">
+        <v>8388608</v>
+      </c>
+      <c r="K20">
+        <v>5436202</v>
+      </c>
+      <c r="L20">
+        <v>563346592</v>
+      </c>
+      <c r="M20">
+        <v>2</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <f>K20/(J20+D20)</f>
+        <v>0.51843662261962886</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21">
+        <v>2097152</v>
+      </c>
+      <c r="E21">
+        <v>1637958</v>
+      </c>
+      <c r="F21">
+        <v>0.1</v>
+      </c>
+      <c r="G21">
+        <v>0.3</v>
+      </c>
+      <c r="H21">
+        <v>64</v>
+      </c>
+      <c r="I21">
+        <v>64</v>
+      </c>
+      <c r="J21">
+        <v>8388608</v>
+      </c>
+      <c r="K21">
+        <v>5477049</v>
+      </c>
+      <c r="L21">
+        <v>334453712</v>
+      </c>
+      <c r="M21">
+        <v>2</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <f>K21/(J21+D21)</f>
+        <v>0.52233209609985354</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22">
+        <v>2097152</v>
+      </c>
+      <c r="E22">
+        <v>2097152</v>
+      </c>
+      <c r="F22">
+        <v>0.1</v>
+      </c>
+      <c r="G22">
+        <v>0.3</v>
+      </c>
+      <c r="H22">
+        <v>64</v>
+      </c>
+      <c r="I22">
+        <v>64</v>
+      </c>
+      <c r="J22">
+        <v>8388608</v>
+      </c>
+      <c r="K22">
+        <v>5495092</v>
+      </c>
+      <c r="L22">
+        <v>338375328</v>
+      </c>
+      <c r="M22">
+        <v>2</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <f>K22/(J22+D22)</f>
+        <v>0.52405281066894527</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23">
+        <v>2097152</v>
+      </c>
+      <c r="E23">
+        <v>1637958</v>
+      </c>
+      <c r="F23">
+        <v>0.1</v>
+      </c>
+      <c r="G23">
+        <v>0.3</v>
+      </c>
+      <c r="H23">
+        <v>16</v>
+      </c>
+      <c r="I23">
+        <v>64</v>
+      </c>
+      <c r="J23">
+        <v>8388608</v>
+      </c>
+      <c r="K23">
+        <v>5552459</v>
+      </c>
+      <c r="L23">
+        <v>184650464</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <f>K23/(J23+D23)</f>
+        <v>0.52952375411987307</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24">
+        <v>2097152</v>
+      </c>
+      <c r="E24">
+        <v>2097152</v>
+      </c>
+      <c r="F24">
+        <v>0.1</v>
+      </c>
+      <c r="G24">
+        <v>0.3</v>
+      </c>
+      <c r="H24">
+        <v>16</v>
+      </c>
+      <c r="I24">
+        <v>64</v>
+      </c>
+      <c r="J24">
+        <v>8388608</v>
+      </c>
+      <c r="K24">
+        <v>5560875</v>
+      </c>
+      <c r="L24">
+        <v>593327504</v>
+      </c>
+      <c r="M24">
+        <v>2</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <f>K24/(J24+D24)</f>
+        <v>0.53032636642456055</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>14</v>
+      </c>
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25">
+        <v>2097152</v>
+      </c>
+      <c r="E25">
+        <v>1898088</v>
+      </c>
+      <c r="F25">
+        <v>0.1</v>
+      </c>
+      <c r="G25">
+        <v>0.3</v>
+      </c>
+      <c r="H25">
+        <v>32</v>
+      </c>
+      <c r="I25">
+        <v>64</v>
+      </c>
+      <c r="J25">
+        <v>8388608</v>
+      </c>
+      <c r="K25">
+        <v>5711297</v>
+      </c>
+      <c r="L25">
+        <v>496623040</v>
+      </c>
+      <c r="M25">
+        <v>2</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <f>K25/(J25+D25)</f>
+        <v>0.5446717262268066</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26">
+        <v>2097152</v>
+      </c>
+      <c r="E26">
+        <v>2097152</v>
+      </c>
+      <c r="F26">
+        <v>0.1</v>
+      </c>
+      <c r="G26">
+        <v>0.3</v>
+      </c>
+      <c r="H26">
+        <v>32</v>
+      </c>
+      <c r="I26">
+        <v>64</v>
+      </c>
+      <c r="J26">
+        <v>8388608</v>
+      </c>
+      <c r="K26">
+        <v>5824099</v>
+      </c>
+      <c r="L26">
+        <v>519423472</v>
+      </c>
+      <c r="M26">
+        <v>2</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <f>K26/(J26+D26)</f>
+        <v>0.55542936325073244</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P27">
+    <sortCondition ref="O2:O27"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFE7D3DE-3FDA-1D45-932A-6BE3FAC6B792}">
+  <dimension ref="A1:P34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2">
+        <v>2097152</v>
+      </c>
+      <c r="E2">
+        <v>2097152</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+      <c r="G2">
+        <v>0.3</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>32</v>
+      </c>
+      <c r="J2">
+        <v>8388608</v>
+      </c>
+      <c r="K2">
+        <v>4261825</v>
+      </c>
+      <c r="L2">
+        <v>338312952</v>
+      </c>
+      <c r="M2">
+        <v>2</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f>K2/(J2+D2)</f>
+        <v>0.40643930435180664</v>
+      </c>
+      <c r="P2">
+        <f>J2/D2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>2097152</v>
+      </c>
+      <c r="E3">
+        <v>1311070</v>
+      </c>
+      <c r="F3">
+        <v>0.1</v>
+      </c>
+      <c r="G3">
+        <v>0.3</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>32</v>
+      </c>
+      <c r="J3">
+        <v>8388608</v>
+      </c>
+      <c r="K3">
+        <v>4631569</v>
+      </c>
+      <c r="L3">
+        <v>468887376</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f>K3/(J3+D3)</f>
+        <v>0.44170083999633791</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>2097152</v>
+      </c>
+      <c r="E4">
+        <v>1311070</v>
+      </c>
+      <c r="F4">
+        <v>0.1</v>
+      </c>
+      <c r="G4">
+        <v>0.3</v>
+      </c>
+      <c r="H4">
+        <v>16</v>
+      </c>
+      <c r="I4">
+        <v>32</v>
+      </c>
+      <c r="J4">
+        <v>8388608</v>
+      </c>
+      <c r="K4">
+        <v>4871722</v>
+      </c>
+      <c r="L4">
+        <v>329523568</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <f>K4/(J4+D4)</f>
+        <v>0.46460361480712892</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>2097152</v>
+      </c>
+      <c r="E5">
+        <v>1311070</v>
+      </c>
+      <c r="F5">
+        <v>0.1</v>
+      </c>
+      <c r="G5">
+        <v>0.3</v>
+      </c>
+      <c r="H5">
+        <v>8</v>
+      </c>
+      <c r="I5">
+        <v>32</v>
+      </c>
+      <c r="J5">
+        <v>8388608</v>
+      </c>
+      <c r="K5">
+        <v>4879992</v>
+      </c>
+      <c r="L5">
+        <v>458131472</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f>K5/(J5+D5)</f>
+        <v>0.46539230346679689</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>2097152</v>
+      </c>
+      <c r="E6">
+        <v>1311070</v>
+      </c>
+      <c r="F6">
+        <v>0.1</v>
+      </c>
+      <c r="G6">
+        <v>0.3</v>
+      </c>
+      <c r="H6">
+        <v>32</v>
+      </c>
+      <c r="I6">
+        <v>32</v>
+      </c>
+      <c r="J6">
+        <v>8388608</v>
+      </c>
+      <c r="K6">
+        <v>4953380</v>
+      </c>
+      <c r="L6">
+        <v>287181952</v>
+      </c>
+      <c r="M6">
+        <v>2</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f>K6/(J6+D6)</f>
+        <v>0.47239112854003906</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>2097152</v>
+      </c>
+      <c r="E7">
+        <v>1638486</v>
+      </c>
+      <c r="F7">
+        <v>0.1</v>
+      </c>
+      <c r="G7">
+        <v>0.3</v>
+      </c>
+      <c r="H7">
+        <v>8</v>
+      </c>
+      <c r="I7">
+        <v>32</v>
+      </c>
+      <c r="J7">
+        <v>8388608</v>
+      </c>
+      <c r="K7">
+        <v>4991825</v>
+      </c>
+      <c r="L7">
+        <v>441126976</v>
+      </c>
+      <c r="M7">
+        <v>2</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f>K7/(J7+D7)</f>
+        <v>0.47605752944946289</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>2097152</v>
+      </c>
+      <c r="E8">
+        <v>1898357</v>
+      </c>
+      <c r="F8">
+        <v>0.1</v>
+      </c>
+      <c r="G8">
+        <v>0.3</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <v>32</v>
+      </c>
+      <c r="J8">
+        <v>8388608</v>
+      </c>
+      <c r="K8">
+        <v>5107895</v>
+      </c>
+      <c r="L8">
+        <v>622357880</v>
+      </c>
+      <c r="M8">
+        <v>2</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f>K8/(J8+D8)</f>
+        <v>0.48712682723999023</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>2097152</v>
+      </c>
+      <c r="E9">
+        <v>2097152</v>
+      </c>
+      <c r="F9">
+        <v>0.1</v>
+      </c>
+      <c r="G9">
+        <v>0.3</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <v>32</v>
+      </c>
+      <c r="J9">
+        <v>8388608</v>
+      </c>
+      <c r="K9">
+        <v>5161871</v>
+      </c>
+      <c r="L9">
+        <v>598122512</v>
+      </c>
+      <c r="M9">
+        <v>2</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f>K9/(J9+D9)</f>
+        <v>0.49227437973022459</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>2097152</v>
+      </c>
+      <c r="E10">
+        <v>1898357</v>
+      </c>
+      <c r="F10">
+        <v>0.1</v>
+      </c>
+      <c r="G10">
+        <v>0.3</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>32</v>
+      </c>
+      <c r="J10">
+        <v>8388608</v>
+      </c>
+      <c r="K10">
+        <v>5218130</v>
+      </c>
+      <c r="L10">
+        <v>338360224</v>
+      </c>
+      <c r="M10">
+        <v>2</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f>K10/(J10+D10)</f>
+        <v>0.49763965606689453</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11">
+        <v>2097152</v>
+      </c>
+      <c r="E11">
+        <v>1638486</v>
+      </c>
+      <c r="F11">
+        <v>0.1</v>
+      </c>
+      <c r="G11">
+        <v>0.3</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>32</v>
+      </c>
+      <c r="J11">
+        <v>8388608</v>
+      </c>
+      <c r="K11">
+        <v>5249753</v>
+      </c>
+      <c r="L11">
+        <v>473752800</v>
+      </c>
+      <c r="M11">
+        <v>2</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f>K11/(J11+D11)</f>
+        <v>0.50065546035766606</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <v>2097152</v>
+      </c>
+      <c r="E12">
+        <v>2097152</v>
+      </c>
+      <c r="F12">
+        <v>0.1</v>
+      </c>
+      <c r="G12">
+        <v>0.3</v>
+      </c>
+      <c r="H12">
+        <v>8</v>
+      </c>
+      <c r="I12">
+        <v>32</v>
+      </c>
+      <c r="J12">
+        <v>8388608</v>
+      </c>
+      <c r="K12">
+        <v>5276076</v>
+      </c>
+      <c r="L12">
+        <v>556187968</v>
+      </c>
+      <c r="M12">
+        <v>2</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f>K12/(J12+D12)</f>
+        <v>0.50316581726074217</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13">
+        <v>2097152</v>
+      </c>
+      <c r="E13">
+        <v>1311070</v>
+      </c>
+      <c r="F13">
+        <v>0.1</v>
+      </c>
+      <c r="G13">
+        <v>0.3</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <v>32</v>
+      </c>
+      <c r="J13">
+        <v>8388608</v>
+      </c>
+      <c r="K13">
+        <v>5310599</v>
+      </c>
+      <c r="L13">
+        <v>176216864</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f>K13/(J13+D13)</f>
+        <v>0.50645818710327151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14">
+        <v>2097152</v>
+      </c>
+      <c r="E14">
+        <v>1311070</v>
+      </c>
+      <c r="F14">
+        <v>0.1</v>
+      </c>
+      <c r="G14">
+        <v>0.3</v>
+      </c>
+      <c r="H14">
+        <v>32</v>
+      </c>
+      <c r="I14">
+        <v>32</v>
+      </c>
+      <c r="J14">
+        <v>8388608</v>
+      </c>
+      <c r="K14">
+        <v>5339838</v>
+      </c>
+      <c r="L14">
+        <v>176226368</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f>K14/(J14+D14)</f>
+        <v>0.50924663543701176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>2097152</v>
+      </c>
+      <c r="E15">
+        <v>2097152</v>
+      </c>
+      <c r="F15">
+        <v>0.1</v>
+      </c>
+      <c r="G15">
+        <v>0.3</v>
+      </c>
+      <c r="H15">
+        <v>16</v>
+      </c>
+      <c r="I15">
+        <v>32</v>
+      </c>
+      <c r="J15">
+        <v>8388608</v>
+      </c>
+      <c r="K15">
+        <v>5352891</v>
+      </c>
+      <c r="L15">
+        <v>400751312</v>
+      </c>
+      <c r="M15">
+        <v>2</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f>K15/(J15+D15)</f>
+        <v>0.51049146652221677</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16">
+        <v>2097152</v>
+      </c>
+      <c r="E16">
+        <v>2097152</v>
+      </c>
+      <c r="F16">
+        <v>0.1</v>
+      </c>
+      <c r="G16">
+        <v>0.3</v>
+      </c>
+      <c r="H16">
+        <v>32</v>
+      </c>
+      <c r="I16">
+        <v>32</v>
+      </c>
+      <c r="J16">
+        <v>8388608</v>
+      </c>
+      <c r="K16">
+        <v>5357183</v>
+      </c>
+      <c r="L16">
+        <v>398752880</v>
+      </c>
+      <c r="M16">
+        <v>2</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f>K16/(J16+D16)</f>
+        <v>0.5109007835388184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>2097152</v>
+      </c>
+      <c r="E17">
+        <v>1638486</v>
+      </c>
+      <c r="F17">
+        <v>0.1</v>
+      </c>
+      <c r="G17">
+        <v>0.3</v>
+      </c>
+      <c r="H17">
+        <v>32</v>
+      </c>
+      <c r="I17">
+        <v>32</v>
+      </c>
+      <c r="J17">
+        <v>8388608</v>
+      </c>
+      <c r="K17">
+        <v>5371168</v>
+      </c>
+      <c r="L17">
+        <v>270224864</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f>K17/(J17+D17)</f>
+        <v>0.51223449707031254</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18">
+        <v>2097152</v>
+      </c>
+      <c r="E18">
+        <v>2097152</v>
+      </c>
+      <c r="F18">
+        <v>0.1</v>
+      </c>
+      <c r="G18">
+        <v>0.3</v>
+      </c>
+      <c r="H18">
+        <v>32</v>
+      </c>
+      <c r="I18">
+        <v>32</v>
+      </c>
+      <c r="J18">
+        <v>8388608</v>
+      </c>
+      <c r="K18">
+        <v>5374370</v>
+      </c>
+      <c r="L18">
+        <v>338312704</v>
+      </c>
+      <c r="M18">
+        <v>2</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <f>K18/(J18+D18)</f>
+        <v>0.51253986358642578</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19">
+        <v>2097152</v>
+      </c>
+      <c r="E19">
+        <v>1638486</v>
+      </c>
+      <c r="F19">
+        <v>0.1</v>
+      </c>
+      <c r="G19">
+        <v>0.3</v>
+      </c>
+      <c r="H19">
+        <v>16</v>
+      </c>
+      <c r="I19">
+        <v>32</v>
+      </c>
+      <c r="J19">
+        <v>8388608</v>
+      </c>
+      <c r="K19">
+        <v>5409859</v>
+      </c>
+      <c r="L19">
+        <v>366964576</v>
+      </c>
+      <c r="M19">
+        <v>2</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <f>K19/(J19+D19)</f>
+        <v>0.51592435836791994</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20">
+        <v>2097152</v>
+      </c>
+      <c r="E20">
+        <v>1311070</v>
+      </c>
+      <c r="F20">
+        <v>0.1</v>
+      </c>
+      <c r="G20">
+        <v>0.3</v>
+      </c>
+      <c r="H20">
+        <v>8</v>
+      </c>
+      <c r="I20">
+        <v>32</v>
+      </c>
+      <c r="J20">
+        <v>8388608</v>
+      </c>
+      <c r="K20">
+        <v>5427777</v>
+      </c>
+      <c r="L20">
+        <v>176366240</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <f>K20/(J20+D20)</f>
+        <v>0.5176331520080566</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21">
+        <v>2097152</v>
+      </c>
+      <c r="E21">
+        <v>1638486</v>
+      </c>
+      <c r="F21">
+        <v>0.1</v>
+      </c>
+      <c r="G21">
+        <v>0.3</v>
+      </c>
+      <c r="H21">
+        <v>16</v>
+      </c>
+      <c r="I21">
+        <v>32</v>
+      </c>
+      <c r="J21">
+        <v>8388608</v>
+      </c>
+      <c r="K21">
+        <v>5486672</v>
+      </c>
+      <c r="L21">
+        <v>184672064</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <f>K21/(J21+D21)</f>
+        <v>0.52324981689453121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22">
+        <v>2097152</v>
+      </c>
+      <c r="E22">
+        <v>2097152</v>
+      </c>
+      <c r="F22">
+        <v>0.1</v>
+      </c>
+      <c r="G22">
+        <v>0.3</v>
+      </c>
+      <c r="H22">
+        <v>8</v>
+      </c>
+      <c r="I22">
+        <v>32</v>
+      </c>
+      <c r="J22">
+        <v>8388608</v>
+      </c>
+      <c r="K22">
+        <v>5507662</v>
+      </c>
+      <c r="L22">
+        <v>338383872</v>
+      </c>
+      <c r="M22">
+        <v>2</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <f>K22/(J22+D22)</f>
+        <v>0.52525157928466792</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23">
+        <v>2097152</v>
+      </c>
+      <c r="E23">
+        <v>2097152</v>
+      </c>
+      <c r="F23">
+        <v>0.1</v>
+      </c>
+      <c r="G23">
+        <v>0.3</v>
+      </c>
+      <c r="H23">
+        <v>4</v>
+      </c>
+      <c r="I23">
+        <v>32</v>
+      </c>
+      <c r="J23">
+        <v>8388608</v>
+      </c>
+      <c r="K23">
+        <v>5522982</v>
+      </c>
+      <c r="L23">
+        <v>338487120</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <f>K23/(J23+D23)</f>
+        <v>0.5267126083374023</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24">
+        <v>2097152</v>
+      </c>
+      <c r="E24">
+        <v>1638486</v>
+      </c>
+      <c r="F24">
+        <v>0.1</v>
+      </c>
+      <c r="G24">
+        <v>0.3</v>
+      </c>
+      <c r="H24">
+        <v>8</v>
+      </c>
+      <c r="I24">
+        <v>32</v>
+      </c>
+      <c r="J24">
+        <v>8388608</v>
+      </c>
+      <c r="K24">
+        <v>5575741</v>
+      </c>
+      <c r="L24">
+        <v>184676096</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <f>K24/(J24+D24)</f>
+        <v>0.53174409866333006</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25">
+        <v>2097152</v>
+      </c>
+      <c r="E25">
+        <v>1898357</v>
+      </c>
+      <c r="F25">
+        <v>0.1</v>
+      </c>
+      <c r="G25">
+        <v>0.3</v>
+      </c>
+      <c r="H25">
+        <v>8</v>
+      </c>
+      <c r="I25">
+        <v>32</v>
+      </c>
+      <c r="J25">
+        <v>8388608</v>
+      </c>
+      <c r="K25">
+        <v>5628169</v>
+      </c>
+      <c r="L25">
+        <v>338382496</v>
+      </c>
+      <c r="M25">
+        <v>2</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <f>K25/(J25+D25)</f>
+        <v>0.53674402236938479</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26">
+        <v>2097152</v>
+      </c>
+      <c r="E26">
+        <v>1311070</v>
+      </c>
+      <c r="F26">
+        <v>0.1</v>
+      </c>
+      <c r="G26">
+        <v>0.3</v>
+      </c>
+      <c r="H26">
+        <v>16</v>
+      </c>
+      <c r="I26">
+        <v>32</v>
+      </c>
+      <c r="J26">
+        <v>8388608</v>
+      </c>
+      <c r="K26">
+        <v>5635200</v>
+      </c>
+      <c r="L26">
+        <v>176197472</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <f>K26/(J26+D26)</f>
+        <v>0.53741455078125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27">
+        <v>2097152</v>
+      </c>
+      <c r="E27">
+        <v>2097152</v>
+      </c>
+      <c r="F27">
+        <v>0.1</v>
+      </c>
+      <c r="G27">
+        <v>0.3</v>
+      </c>
+      <c r="H27">
+        <v>16</v>
+      </c>
+      <c r="I27">
+        <v>32</v>
+      </c>
+      <c r="J27">
+        <v>8388608</v>
+      </c>
+      <c r="K27">
+        <v>5692287</v>
+      </c>
+      <c r="L27">
+        <v>338447208</v>
+      </c>
+      <c r="M27">
+        <v>2</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <f>K27/(J27+D27)</f>
+        <v>0.54285879135131831</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28">
+        <v>2097152</v>
+      </c>
+      <c r="E28">
+        <v>1898357</v>
+      </c>
+      <c r="F28">
+        <v>0.1</v>
+      </c>
+      <c r="G28">
+        <v>0.3</v>
+      </c>
+      <c r="H28">
+        <v>16</v>
+      </c>
+      <c r="I28">
+        <v>32</v>
+      </c>
+      <c r="J28">
+        <v>8388608</v>
+      </c>
+      <c r="K28">
+        <v>5755442</v>
+      </c>
+      <c r="L28">
+        <v>486911064</v>
+      </c>
+      <c r="M28">
+        <v>2</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <f>K28/(J28+D28)</f>
+        <v>0.54888172149658199</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>17</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29">
+        <v>2097152</v>
+      </c>
+      <c r="E29">
+        <v>1638486</v>
+      </c>
+      <c r="F29">
+        <v>0.1</v>
+      </c>
+      <c r="G29">
+        <v>0.3</v>
+      </c>
+      <c r="H29">
+        <v>4</v>
+      </c>
+      <c r="I29">
+        <v>32</v>
+      </c>
+      <c r="J29">
+        <v>8388608</v>
+      </c>
+      <c r="K29">
+        <v>5778231</v>
+      </c>
+      <c r="L29">
+        <v>184640384</v>
+      </c>
+      <c r="M29">
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <f>K29/(J29+D29)</f>
+        <v>0.55105504989624021</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>13</v>
+      </c>
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30">
+        <v>2097152</v>
+      </c>
+      <c r="E30">
+        <v>1898357</v>
+      </c>
+      <c r="F30">
+        <v>0.1</v>
+      </c>
+      <c r="G30">
+        <v>0.3</v>
+      </c>
+      <c r="H30">
+        <v>16</v>
+      </c>
+      <c r="I30">
+        <v>32</v>
+      </c>
+      <c r="J30">
+        <v>8388608</v>
+      </c>
+      <c r="K30">
+        <v>5791378</v>
+      </c>
+      <c r="L30">
+        <v>338452704</v>
+      </c>
+      <c r="M30">
+        <v>2</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <f>K30/(J30+D30)</f>
+        <v>0.55230884552001958</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>12</v>
+      </c>
+      <c r="B31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31">
+        <v>2097152</v>
+      </c>
+      <c r="E31">
+        <v>1898357</v>
+      </c>
+      <c r="F31">
+        <v>0.1</v>
+      </c>
+      <c r="G31">
+        <v>0.3</v>
+      </c>
+      <c r="H31">
+        <v>8</v>
+      </c>
+      <c r="I31">
+        <v>32</v>
+      </c>
+      <c r="J31">
+        <v>8388608</v>
+      </c>
+      <c r="K31">
+        <v>5799659</v>
+      </c>
+      <c r="L31">
+        <v>560818920</v>
+      </c>
+      <c r="M31">
+        <v>2</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <f>K31/(J31+D31)</f>
+        <v>0.55309858322143557</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>15</v>
+      </c>
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32">
+        <v>2097152</v>
+      </c>
+      <c r="E32">
+        <v>1898357</v>
+      </c>
+      <c r="F32">
+        <v>0.1</v>
+      </c>
+      <c r="G32">
+        <v>0.3</v>
+      </c>
+      <c r="H32">
+        <v>32</v>
+      </c>
+      <c r="I32">
+        <v>32</v>
+      </c>
+      <c r="J32">
+        <v>8388608</v>
+      </c>
+      <c r="K32">
+        <v>5813279</v>
+      </c>
+      <c r="L32">
+        <v>338357440</v>
+      </c>
+      <c r="M32">
+        <v>2</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <f>K32/(J32+D32)</f>
+        <v>0.55439748764038088</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>23</v>
+      </c>
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33">
+        <v>2097152</v>
+      </c>
+      <c r="E33">
+        <v>1638486</v>
+      </c>
+      <c r="F33">
+        <v>0.1</v>
+      </c>
+      <c r="G33">
+        <v>0.3</v>
+      </c>
+      <c r="H33">
+        <v>32</v>
+      </c>
+      <c r="I33">
+        <v>32</v>
+      </c>
+      <c r="J33">
+        <v>8388608</v>
+      </c>
+      <c r="K33">
+        <v>5841973</v>
+      </c>
+      <c r="L33">
+        <v>184642688</v>
+      </c>
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <f>K33/(J33+D33)</f>
+        <v>0.557133960723877</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>16</v>
+      </c>
+      <c r="B34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34">
+        <v>2097152</v>
+      </c>
+      <c r="E34">
+        <v>1898357</v>
+      </c>
+      <c r="F34">
+        <v>0.1</v>
+      </c>
+      <c r="G34">
+        <v>0.3</v>
+      </c>
+      <c r="H34">
+        <v>32</v>
+      </c>
+      <c r="I34">
+        <v>32</v>
+      </c>
+      <c r="J34">
+        <v>8388608</v>
+      </c>
+      <c r="K34">
+        <v>5941913</v>
+      </c>
+      <c r="L34">
+        <v>394030312</v>
+      </c>
+      <c r="M34">
+        <v>2</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <f>K34/(J34+D34)</f>
+        <v>0.56666498184204106</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O35">
+    <sortCondition ref="O2:O35"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>